<commit_message>
[Modified]: Activity Bar Chart
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Báo Cáo Team/General/activity_bar_chart_2.xlsx
+++ b/ToDoApp-Doc/Báo Cáo Team/General/activity_bar_chart_2.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="231">
   <si>
     <t>Create a Gantt Chart in this worksheet.
 Enter title of this project in cell B1. 
@@ -737,6 +737,15 @@
   <si>
     <t>MANAGE SUBTASK</t>
   </si>
+  <si>
+    <t>Pause music</t>
+  </si>
+  <si>
+    <t>Continues music</t>
+  </si>
+  <si>
+    <t>Break music</t>
+  </si>
 </sst>
 </file>
 
@@ -1284,7 +1293,240 @@
     <cellStyle name="Title 2" xfId="4"/>
     <cellStyle name="zHiddenText" xfId="3"/>
   </cellStyles>
-  <dxfs count="151">
+  <dxfs count="161">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4191,69 +4433,6 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -4305,9 +4484,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Gantt Table Style" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="150"/>
-      <tableStyleElement type="headerRow" dxfId="149"/>
-      <tableStyleElement type="firstRowStripe" dxfId="148"/>
+      <tableStyleElement type="wholeTable" dxfId="160"/>
+      <tableStyleElement type="headerRow" dxfId="159"/>
+      <tableStyleElement type="firstRowStripe" dxfId="158"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -4343,14 +4522,14 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Milestones" displayName="Milestones" ref="B7:I170" totalsRowShown="0">
   <tableColumns count="8">
-    <tableColumn id="1" name="Functions" dataDxfId="147"/>
-    <tableColumn id="2" name="Category" dataDxfId="146"/>
-    <tableColumn id="9" name="Milestone" dataDxfId="145"/>
-    <tableColumn id="3" name="Assigned To" dataDxfId="144"/>
-    <tableColumn id="10" name="Story Point" dataDxfId="143"/>
+    <tableColumn id="1" name="Functions" dataDxfId="16"/>
+    <tableColumn id="2" name="Category" dataDxfId="15"/>
+    <tableColumn id="9" name="Milestone" dataDxfId="14"/>
+    <tableColumn id="3" name="Assigned To" dataDxfId="13"/>
+    <tableColumn id="10" name="Story Point" dataDxfId="12"/>
     <tableColumn id="4" name="Progress"/>
-    <tableColumn id="5" name="Start" dataDxfId="142" dataCellStyle="Date"/>
-    <tableColumn id="6" name="End" dataDxfId="141" dataCellStyle="Comma [0]"/>
+    <tableColumn id="5" name="Start" dataDxfId="11" dataCellStyle="Date"/>
+    <tableColumn id="6" name="End" dataDxfId="10" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="Gantt Table Style" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -4629,9 +4808,9 @@
   </sheetPr>
   <dimension ref="A1:FM172"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane xSplit="9" topLeftCell="AW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane xSplit="9" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6484,13 +6663,13 @@
       <c r="BE10" s="60"/>
       <c r="BF10" s="60"/>
       <c r="BG10" s="60"/>
-      <c r="BH10" s="34"/>
-      <c r="BI10" s="34"/>
-      <c r="BJ10" s="34"/>
-      <c r="BK10" s="34"/>
-      <c r="BL10" s="34"/>
-      <c r="BM10" s="34"/>
-      <c r="BN10" s="34"/>
+      <c r="BH10" s="60"/>
+      <c r="BI10" s="60"/>
+      <c r="BJ10" s="60"/>
+      <c r="BK10" s="60"/>
+      <c r="BL10" s="60"/>
+      <c r="BM10" s="60"/>
+      <c r="BN10" s="60"/>
       <c r="BO10" s="34"/>
       <c r="BP10" s="34"/>
       <c r="BQ10" s="34"/>
@@ -6783,13 +6962,13 @@
       <c r="BE12" s="60"/>
       <c r="BF12" s="60"/>
       <c r="BG12" s="60"/>
-      <c r="BH12" s="34"/>
-      <c r="BI12" s="34"/>
-      <c r="BJ12" s="34"/>
-      <c r="BK12" s="34"/>
-      <c r="BL12" s="34"/>
-      <c r="BM12" s="34"/>
-      <c r="BN12" s="34"/>
+      <c r="BH12" s="60"/>
+      <c r="BI12" s="60"/>
+      <c r="BJ12" s="60"/>
+      <c r="BK12" s="60"/>
+      <c r="BL12" s="60"/>
+      <c r="BM12" s="60"/>
+      <c r="BN12" s="60"/>
       <c r="BO12" s="34"/>
       <c r="BP12" s="34"/>
       <c r="BQ12" s="34"/>
@@ -9102,8 +9281,8 @@
       <c r="AV28" s="34"/>
       <c r="AW28" s="34"/>
       <c r="AX28" s="34"/>
-      <c r="AY28" s="60"/>
-      <c r="AZ28" s="60"/>
+      <c r="AY28" s="34"/>
+      <c r="AZ28" s="34"/>
       <c r="BA28" s="60"/>
       <c r="BB28" s="60"/>
       <c r="BC28" s="60"/>
@@ -9111,13 +9290,13 @@
       <c r="BE28" s="60"/>
       <c r="BF28" s="60"/>
       <c r="BG28" s="60"/>
-      <c r="BH28" s="60"/>
-      <c r="BI28" s="60"/>
-      <c r="BJ28" s="60"/>
-      <c r="BK28" s="60"/>
-      <c r="BL28" s="60"/>
-      <c r="BM28" s="60"/>
-      <c r="BN28" s="60"/>
+      <c r="BH28" s="34"/>
+      <c r="BI28" s="34"/>
+      <c r="BJ28" s="34"/>
+      <c r="BK28" s="34"/>
+      <c r="BL28" s="34"/>
+      <c r="BM28" s="34"/>
+      <c r="BN28" s="34"/>
       <c r="BO28" s="34"/>
       <c r="BP28" s="34"/>
       <c r="BQ28" s="34"/>
@@ -27404,9 +27583,15 @@
       <c r="FM141" s="27"/>
     </row>
     <row r="142" spans="1:169" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B142" s="42"/>
-      <c r="C142" s="38"/>
-      <c r="D142" s="45"/>
+      <c r="B142" s="49" t="s">
+        <v>228</v>
+      </c>
+      <c r="C142" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D142" s="45" t="s">
+        <v>143</v>
+      </c>
       <c r="E142" s="38"/>
       <c r="F142" s="45"/>
       <c r="G142" s="31"/>
@@ -27576,9 +27761,15 @@
       <c r="FM142" s="27"/>
     </row>
     <row r="143" spans="1:169" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B143" s="42"/>
-      <c r="C143" s="38"/>
-      <c r="D143" s="45"/>
+      <c r="B143" s="49" t="s">
+        <v>229</v>
+      </c>
+      <c r="C143" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D143" s="45" t="s">
+        <v>143</v>
+      </c>
       <c r="E143" s="38"/>
       <c r="F143" s="45"/>
       <c r="G143" s="31"/>
@@ -27746,9 +27937,15 @@
     </row>
     <row r="144" spans="1:169" s="41" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="28"/>
-      <c r="B144" s="42"/>
-      <c r="C144" s="38"/>
-      <c r="D144" s="45"/>
+      <c r="B144" s="49" t="s">
+        <v>230</v>
+      </c>
+      <c r="C144" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D144" s="45" t="s">
+        <v>143</v>
+      </c>
       <c r="E144" s="38"/>
       <c r="F144" s="45"/>
       <c r="G144" s="31"/>
@@ -30029,7 +30226,7 @@
     <mergeCell ref="DT2:DW2"/>
   </mergeCells>
   <conditionalFormatting sqref="G147:G170 G7:G8 G30:G144 G13:G27">
-    <cfRule type="dataBar" priority="211">
+    <cfRule type="dataBar" priority="231">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -30043,44 +30240,44 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM5:FJ8">
-    <cfRule type="expression" dxfId="140" priority="210">
+    <cfRule type="expression" dxfId="157" priority="230">
       <formula>AND(TODAY()&gt;=EM$5,TODAY()&lt;EN$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK5:FK6">
-    <cfRule type="expression" dxfId="139" priority="213">
+    <cfRule type="expression" dxfId="156" priority="233">
       <formula>AND(TODAY()&gt;=FK$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H171:I171 J93 DV92 DV95">
-    <cfRule type="expression" dxfId="138" priority="214">
+    <cfRule type="expression" dxfId="155" priority="234">
       <formula>AND(TODAY()&gt;=K$4,TODAY()&lt;L$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H171:I171 J93 DV92 DV95">
-    <cfRule type="expression" dxfId="137" priority="215" stopIfTrue="1">
+    <cfRule type="expression" dxfId="154" priority="235" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",K$4&gt;=#REF!,K$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="216" stopIfTrue="1">
+    <cfRule type="expression" dxfId="153" priority="236" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",K$4&gt;=#REF!,K$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="135" priority="217" stopIfTrue="1">
+    <cfRule type="expression" dxfId="152" priority="237" stopIfTrue="1">
       <formula>AND(#REF!="On Track",K$4&gt;=#REF!,K$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="134" priority="218" stopIfTrue="1">
+    <cfRule type="expression" dxfId="151" priority="238" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",K$4&gt;=#REF!,K$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="133" priority="219" stopIfTrue="1">
+    <cfRule type="expression" dxfId="150" priority="239" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,K$4&gt;=#REF!,K$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK7:FK8">
-    <cfRule type="expression" dxfId="132" priority="220">
+    <cfRule type="expression" dxfId="149" priority="240">
       <formula>AND(TODAY()&gt;=FK$5,TODAY()&lt;#REF!)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G145:G146">
-    <cfRule type="dataBar" priority="208">
+    <cfRule type="dataBar" priority="228">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -30094,260 +30291,260 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM8:FK8">
-    <cfRule type="expression" dxfId="131" priority="222" stopIfTrue="1">
+    <cfRule type="expression" dxfId="148" priority="242" stopIfTrue="1">
       <formula>AND($C8="Low Risk",EM$5&gt;=$H8,EM$5&lt;=$H8+$I8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="130" priority="223" stopIfTrue="1">
+    <cfRule type="expression" dxfId="147" priority="243" stopIfTrue="1">
       <formula>AND($C8="High Risk",EM$5&gt;=$H8,EM$5&lt;=$H8+$I8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="129" priority="224" stopIfTrue="1">
+    <cfRule type="expression" dxfId="146" priority="244" stopIfTrue="1">
       <formula>AND($C8="On Track",EM$5&gt;=$H8,EM$5&lt;=$H8+$I8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="128" priority="225" stopIfTrue="1">
+    <cfRule type="expression" dxfId="145" priority="245" stopIfTrue="1">
       <formula>AND($C8="Med Risk",EM$5&gt;=$H8,EM$5&lt;=$H8+$I8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="127" priority="226" stopIfTrue="1">
+    <cfRule type="expression" dxfId="144" priority="246" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,EM$5&gt;=$H8,EM$5&lt;=$H8+$I8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EL4:EL8">
-    <cfRule type="expression" dxfId="126" priority="227">
+    <cfRule type="expression" dxfId="143" priority="247">
       <formula>AND(TODAY()&gt;=EL$4,TODAY()&lt;EM$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DW7:EK7 DV121:DV123 DV125:DV127 DV129:DV131 DV133:DV135 DV137:DV139 DV141:DV143 DU145:DV147 DU149:DV150 DU144 DU148 DV93:DV94 K4:S5 DR4:EK6 DR8:EK8 DV96:DV119 DR144:DT150 K6 K8:S8 K13:DV13 DV84:DV91 DR84:DU143 BW67:BZ67 CB67:DI67 K67:BU68 BY68:DI68 K69:DI150 K30:DI66 DR30:DV83 DR14:DV27 K14:DI27">
-    <cfRule type="expression" dxfId="125" priority="228">
+    <cfRule type="expression" dxfId="142" priority="248">
       <formula>AND(TODAY()&gt;=K$4,TODAY()&lt;L$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM4:FK4">
-    <cfRule type="expression" dxfId="124" priority="229">
+    <cfRule type="expression" dxfId="141" priority="249">
       <formula>AND(EM$5&lt;=EOMONTH($K$4,2),EM$5&gt;EOMONTH($K$4,0),EM$5&gt;EOMONTH($K$4,1))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM4:FK4">
-    <cfRule type="expression" dxfId="123" priority="230">
+    <cfRule type="expression" dxfId="140" priority="250">
       <formula>AND(EM$5&lt;=EOMONTH($K$4,1),EM$5&gt;EOMONTH($K$4,0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DW7:EL7 DV99 DJ15:DV26 DV84:DV90 DJ84:DU143 DJ29:DV83">
-    <cfRule type="expression" dxfId="122" priority="231" stopIfTrue="1">
+    <cfRule type="expression" dxfId="139" priority="251" stopIfTrue="1">
       <formula>AND($C8="Low Risk",DJ$4&gt;=$H8,DJ$4&lt;=$H8+$I8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="121" priority="232" stopIfTrue="1">
+    <cfRule type="expression" dxfId="138" priority="252" stopIfTrue="1">
       <formula>AND($C8="High Risk",DJ$4&gt;=$H8,DJ$4&lt;=$H8+$I8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="120" priority="233" stopIfTrue="1">
+    <cfRule type="expression" dxfId="137" priority="253" stopIfTrue="1">
       <formula>AND($C8="On Track",DJ$4&gt;=$H8,DJ$4&lt;=$H8+$I8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="234" stopIfTrue="1">
+    <cfRule type="expression" dxfId="136" priority="254" stopIfTrue="1">
       <formula>AND($C8="Med Risk",DJ$4&gt;=$H8,DJ$4&lt;=$H8+$I8-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="235" stopIfTrue="1">
+    <cfRule type="expression" dxfId="135" priority="255" stopIfTrue="1">
       <formula>AND(LEN($C8)=0,DJ$4&gt;=$H8,DJ$4&lt;=$H8+$I8-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DV91">
-    <cfRule type="expression" dxfId="117" priority="236" stopIfTrue="1">
+    <cfRule type="expression" dxfId="134" priority="256" stopIfTrue="1">
       <formula>AND($C112="Low Risk",DV$4&gt;=$H112,DV$4&lt;=$H112+$I112-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="237" stopIfTrue="1">
+    <cfRule type="expression" dxfId="133" priority="257" stopIfTrue="1">
       <formula>AND($C112="High Risk",DV$4&gt;=$H112,DV$4&lt;=$H112+$I112-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="238" stopIfTrue="1">
+    <cfRule type="expression" dxfId="132" priority="258" stopIfTrue="1">
       <formula>AND($C112="On Track",DV$4&gt;=$H112,DV$4&lt;=$H112+$I112-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="114" priority="239" stopIfTrue="1">
+    <cfRule type="expression" dxfId="131" priority="259" stopIfTrue="1">
       <formula>AND($C112="Med Risk",DV$4&gt;=$H112,DV$4&lt;=$H112+$I112-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="113" priority="240" stopIfTrue="1">
+    <cfRule type="expression" dxfId="130" priority="260" stopIfTrue="1">
       <formula>AND(LEN($C112)=0,DV$4&gt;=$H112,DV$4&lt;=$H112+$I112-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DV121 DV125 DV129 DV133 DV137 DV141 DU145:DV145 DU149:DV149 DV100:DV117">
-    <cfRule type="expression" dxfId="112" priority="246" stopIfTrue="1">
+    <cfRule type="expression" dxfId="129" priority="266" stopIfTrue="1">
       <formula>AND($C178="Low Risk",DU$4&gt;=$H178,DU$4&lt;=$H178+$I178-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="111" priority="247" stopIfTrue="1">
+    <cfRule type="expression" dxfId="128" priority="267" stopIfTrue="1">
       <formula>AND($C178="High Risk",DU$4&gt;=$H178,DU$4&lt;=$H178+$I178-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="110" priority="248" stopIfTrue="1">
+    <cfRule type="expression" dxfId="127" priority="268" stopIfTrue="1">
       <formula>AND($C178="On Track",DU$4&gt;=$H178,DU$4&lt;=$H178+$I178-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="109" priority="249" stopIfTrue="1">
+    <cfRule type="expression" dxfId="126" priority="269" stopIfTrue="1">
       <formula>AND($C178="Med Risk",DU$4&gt;=$H178,DU$4&lt;=$H178+$I178-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="108" priority="250" stopIfTrue="1">
+    <cfRule type="expression" dxfId="125" priority="270" stopIfTrue="1">
       <formula>AND(LEN($C178)=0,DU$4&gt;=$H178,DU$4&lt;=$H178+$I178-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DU150:DV150 DU144 DU148 DV122:DV123 DV126:DV127 DV130:DV131 DV134:DV135 DV138:DV139 DV142:DV143 DU146:DV147 DJ144:DT150 DV118:DV119">
-    <cfRule type="expression" dxfId="107" priority="251" stopIfTrue="1">
+    <cfRule type="expression" dxfId="124" priority="271" stopIfTrue="1">
       <formula>AND($C184="Low Risk",DJ$4&gt;=$H184,DJ$4&lt;=$H184+$I184-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="106" priority="252" stopIfTrue="1">
+    <cfRule type="expression" dxfId="123" priority="272" stopIfTrue="1">
       <formula>AND($C184="High Risk",DJ$4&gt;=$H184,DJ$4&lt;=$H184+$I184-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="105" priority="253" stopIfTrue="1">
+    <cfRule type="expression" dxfId="122" priority="273" stopIfTrue="1">
       <formula>AND($C184="On Track",DJ$4&gt;=$H184,DJ$4&lt;=$H184+$I184-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="254" stopIfTrue="1">
+    <cfRule type="expression" dxfId="121" priority="274" stopIfTrue="1">
       <formula>AND($C184="Med Risk",DJ$4&gt;=$H184,DJ$4&lt;=$H184+$I184-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="255" stopIfTrue="1">
+    <cfRule type="expression" dxfId="120" priority="275" stopIfTrue="1">
       <formula>AND(LEN($C184)=0,DJ$4&gt;=$H184,DJ$4&lt;=$H184+$I184-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DV96:DV98 DV93:DV94">
-    <cfRule type="expression" dxfId="102" priority="256" stopIfTrue="1">
+    <cfRule type="expression" dxfId="119" priority="276" stopIfTrue="1">
       <formula>AND($C172="Low Risk",DV$4&gt;=$H172,DV$4&lt;=$H172+$I172-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="101" priority="257" stopIfTrue="1">
+    <cfRule type="expression" dxfId="118" priority="277" stopIfTrue="1">
       <formula>AND($C172="High Risk",DV$4&gt;=$H172,DV$4&lt;=$H172+$I172-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="258" stopIfTrue="1">
+    <cfRule type="expression" dxfId="117" priority="278" stopIfTrue="1">
       <formula>AND($C172="On Track",DV$4&gt;=$H172,DV$4&lt;=$H172+$I172-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="259" stopIfTrue="1">
+    <cfRule type="expression" dxfId="116" priority="279" stopIfTrue="1">
       <formula>AND($C172="Med Risk",DV$4&gt;=$H172,DV$4&lt;=$H172+$I172-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="260" stopIfTrue="1">
+    <cfRule type="expression" dxfId="115" priority="280" stopIfTrue="1">
       <formula>AND(LEN($C172)=0,DV$4&gt;=$H172,DV$4&lt;=$H172+$I172-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DO7:DV7 K7:CO7">
-    <cfRule type="expression" dxfId="97" priority="190">
+    <cfRule type="expression" dxfId="114" priority="210">
       <formula>K$6=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DN4:DQ6 DN8:DQ8 DN30:DQ150 DN14:DQ27">
-    <cfRule type="expression" dxfId="96" priority="307">
+    <cfRule type="expression" dxfId="113" priority="327">
       <formula>AND(TODAY()&gt;=DN$4,TODAY()&lt;DS$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DJ4:DM6 DJ8:DM8 CZ27:DI27 DJ30:DM150 DJ14:DM27">
-    <cfRule type="expression" dxfId="95" priority="459">
+    <cfRule type="expression" dxfId="112" priority="479">
       <formula>AND(TODAY()&gt;=CZ$4,TODAY()&lt;DI$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DF4:DI5 DF8:DI8">
-    <cfRule type="expression" dxfId="94" priority="611">
+    <cfRule type="expression" dxfId="111" priority="631">
       <formula>AND(TODAY()&gt;=DF$4,TODAY()&lt;DS$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DB4:DE5 DB8:DE8">
-    <cfRule type="expression" dxfId="93" priority="763">
+    <cfRule type="expression" dxfId="110" priority="783">
       <formula>AND(TODAY()&gt;=DB$4,TODAY()&lt;DS$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BO4:CG5 BO8:CG8">
-    <cfRule type="expression" dxfId="92" priority="915">
+    <cfRule type="expression" dxfId="109" priority="935">
       <formula>AND(TODAY()&gt;=BO$4,TODAY()&lt;DT$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CX4:DA5 CX8:DA8">
-    <cfRule type="expression" dxfId="91" priority="130">
+    <cfRule type="expression" dxfId="108" priority="150">
       <formula>AND(TODAY()&gt;=CX$4,TODAY()&lt;CY$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP7:DN7">
-    <cfRule type="expression" dxfId="90" priority="114">
+    <cfRule type="expression" dxfId="107" priority="134">
       <formula>CP$6=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CT4:CW5 CT8:CW8">
-    <cfRule type="expression" dxfId="89" priority="168">
+    <cfRule type="expression" dxfId="106" priority="188">
       <formula>AND(TODAY()&gt;=CT$4,TODAY()&lt;CY$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CP4:CS5 CP8:CS8 CP6">
-    <cfRule type="expression" dxfId="88" priority="175">
+    <cfRule type="expression" dxfId="105" priority="195">
       <formula>AND(TODAY()&gt;=CP$4,TODAY()&lt;CY$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL4:CO5 CL8:CO8">
-    <cfRule type="expression" dxfId="87" priority="182">
+    <cfRule type="expression" dxfId="104" priority="202">
       <formula>AND(TODAY()&gt;=CL$4,TODAY()&lt;CY$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CH4:CK5 CH8:CK8">
-    <cfRule type="expression" dxfId="86" priority="189">
+    <cfRule type="expression" dxfId="103" priority="209">
       <formula>AND(TODAY()&gt;=CH$4,TODAY()&lt;CY$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BM4:BN5 BM8:BN8">
-    <cfRule type="expression" dxfId="85" priority="1243">
+    <cfRule type="expression" dxfId="102" priority="1263">
       <formula>AND(TODAY()&gt;=BM$4,TODAY()&lt;DS$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T4:BL5 T8:BL8 AG6 BL6">
-    <cfRule type="expression" dxfId="84" priority="1422">
+    <cfRule type="expression" dxfId="101" priority="1442">
       <formula>AND(TODAY()&gt;=T$4,TODAY()&lt;DR$4)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BW67:BZ67 CB67:DI67 BY68:DI68 K15:DI26 K67:BU68 K69:DI150 K28:DV28 K29:DI66">
-    <cfRule type="expression" dxfId="83" priority="1468" stopIfTrue="1">
+  <conditionalFormatting sqref="BW67:BZ67 CB67:DI67 BY68:DI68 K15:DI26 K67:BU68 K69:DI150 K29:DI66 K28:DV28">
+    <cfRule type="expression" dxfId="100" priority="1488" stopIfTrue="1">
       <formula>AND($C16="Low Risk",K$4&gt;=$H15,K$4&lt;=$H15+$I16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="1469" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="1489" stopIfTrue="1">
       <formula>AND($C16="High Risk",K$4&gt;=$H15,K$4&lt;=$H15+$I16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="1470" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="1490" stopIfTrue="1">
       <formula>AND($C16="On Track",K$4&gt;=$H15,K$4&lt;=$H15+$I16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="1471" stopIfTrue="1">
+    <cfRule type="expression" dxfId="97" priority="1491" stopIfTrue="1">
       <formula>AND($C16="Med Risk",K$4&gt;=$H15,K$4&lt;=$H15+$I16-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="79" priority="1472" stopIfTrue="1">
+    <cfRule type="expression" dxfId="96" priority="1492" stopIfTrue="1">
       <formula>AND(LEN($C16)=0,K$4&gt;=$H15,K$4&lt;=$H15+$I16-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV67">
-    <cfRule type="expression" dxfId="78" priority="1479">
+    <cfRule type="expression" dxfId="95" priority="1499">
       <formula>AND(TODAY()&gt;=CA$4,TODAY()&lt;CB$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV67">
-    <cfRule type="expression" dxfId="77" priority="1635" stopIfTrue="1">
+    <cfRule type="expression" dxfId="94" priority="1655" stopIfTrue="1">
       <formula>AND($C68="Low Risk",CA$4&gt;=$H67,CA$4&lt;=$H67+$I68-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="1636" stopIfTrue="1">
+    <cfRule type="expression" dxfId="93" priority="1656" stopIfTrue="1">
       <formula>AND($C68="High Risk",CA$4&gt;=$H67,CA$4&lt;=$H67+$I68-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="1637" stopIfTrue="1">
+    <cfRule type="expression" dxfId="92" priority="1657" stopIfTrue="1">
       <formula>AND($C68="On Track",CA$4&gt;=$H67,CA$4&lt;=$H67+$I68-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="1638" stopIfTrue="1">
+    <cfRule type="expression" dxfId="91" priority="1658" stopIfTrue="1">
       <formula>AND($C68="Med Risk",CA$4&gt;=$H67,CA$4&lt;=$H67+$I68-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="73" priority="1639" stopIfTrue="1">
+    <cfRule type="expression" dxfId="90" priority="1659" stopIfTrue="1">
       <formula>AND(LEN($C68)=0,CA$4&gt;=$H67,CA$4&lt;=$H67+$I68-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV68:BW68">
-    <cfRule type="expression" dxfId="72" priority="1641">
+    <cfRule type="expression" dxfId="89" priority="1661">
       <formula>AND(TODAY()&gt;=BW$4,TODAY()&lt;BX$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BV68:BW68">
-    <cfRule type="expression" dxfId="71" priority="1802" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="1822" stopIfTrue="1">
       <formula>AND($C69="Low Risk",BW$4&gt;=$H68,BW$4&lt;=$H68+$I69-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="1803" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="1823" stopIfTrue="1">
       <formula>AND($C69="High Risk",BW$4&gt;=$H68,BW$4&lt;=$H68+$I69-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="1804" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="1824" stopIfTrue="1">
       <formula>AND($C69="On Track",BW$4&gt;=$H68,BW$4&lt;=$H68+$I69-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="1805" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="1825" stopIfTrue="1">
       <formula>AND($C69="Med Risk",BW$4&gt;=$H68,BW$4&lt;=$H68+$I69-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="67" priority="1806" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="1826" stopIfTrue="1">
       <formula>AND(LEN($C69)=0,BW$4&gt;=$H68,BW$4&lt;=$H68+$I69-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G11">
-    <cfRule type="dataBar" priority="106">
+    <cfRule type="dataBar" priority="126">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -30361,46 +30558,46 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:DV11">
-    <cfRule type="expression" dxfId="66" priority="107">
+    <cfRule type="expression" dxfId="83" priority="127">
       <formula>AND(TODAY()&gt;=K$4,TODAY()&lt;L$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11:DV11">
-    <cfRule type="expression" dxfId="65" priority="108" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="128" stopIfTrue="1">
       <formula>AND($C12="Low Risk",K$4&gt;=$H11,K$4&lt;=$H11+$I12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="109" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="129" stopIfTrue="1">
       <formula>AND($C12="High Risk",K$4&gt;=$H11,K$4&lt;=$H11+$I12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="110" stopIfTrue="1">
+    <cfRule type="expression" dxfId="80" priority="130" stopIfTrue="1">
       <formula>AND($C12="On Track",K$4&gt;=$H11,K$4&lt;=$H11+$I12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="111" stopIfTrue="1">
+    <cfRule type="expression" dxfId="79" priority="131" stopIfTrue="1">
       <formula>AND($C12="Med Risk",K$4&gt;=$H11,K$4&lt;=$H11+$I12-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="112" stopIfTrue="1">
+    <cfRule type="expression" dxfId="78" priority="132" stopIfTrue="1">
       <formula>AND(LEN($C12)=0,K$4&gt;=$H11,K$4&lt;=$H11+$I12-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8:EL8">
-    <cfRule type="expression" dxfId="60" priority="2342" stopIfTrue="1">
+    <cfRule type="expression" dxfId="77" priority="2362" stopIfTrue="1">
       <formula>AND($C13="Low Risk",K$4&gt;=#REF!,K$4&lt;=#REF!+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="59" priority="2343" stopIfTrue="1">
+    <cfRule type="expression" dxfId="76" priority="2363" stopIfTrue="1">
       <formula>AND($C13="High Risk",K$4&gt;=#REF!,K$4&lt;=#REF!+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="2344" stopIfTrue="1">
+    <cfRule type="expression" dxfId="75" priority="2364" stopIfTrue="1">
       <formula>AND($C13="On Track",K$4&gt;=#REF!,K$4&lt;=#REF!+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="2345" stopIfTrue="1">
+    <cfRule type="expression" dxfId="74" priority="2365" stopIfTrue="1">
       <formula>AND($C13="Med Risk",K$4&gt;=#REF!,K$4&lt;=#REF!+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="2346" stopIfTrue="1">
+    <cfRule type="expression" dxfId="73" priority="2366" stopIfTrue="1">
       <formula>AND(LEN($C13)=0,K$4&gt;=#REF!,K$4&lt;=#REF!+$I13-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="dataBar" priority="54">
+    <cfRule type="dataBar" priority="74">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -30414,7 +30611,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="dataBar" priority="69">
+    <cfRule type="dataBar" priority="89">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -30428,78 +30625,78 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:DV9">
-    <cfRule type="expression" dxfId="55" priority="70">
+    <cfRule type="expression" dxfId="72" priority="90">
       <formula>AND(TODAY()&gt;=K$4,TODAY()&lt;L$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:DV9">
-    <cfRule type="expression" dxfId="54" priority="71" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="91" stopIfTrue="1">
       <formula>AND($C10="Low Risk",K$4&gt;=$H9,K$4&lt;=$H9+$I10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="72" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="92" stopIfTrue="1">
       <formula>AND($C10="High Risk",K$4&gt;=$H9,K$4&lt;=$H9+$I10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="93" stopIfTrue="1">
       <formula>AND($C10="On Track",K$4&gt;=$H9,K$4&lt;=$H9+$I10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="74" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="94" stopIfTrue="1">
       <formula>AND($C10="Med Risk",K$4&gt;=$H9,K$4&lt;=$H9+$I10-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="95" stopIfTrue="1">
       <formula>AND(LEN($C10)=0,K$4&gt;=$H9,K$4&lt;=$H9+$I10-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DR10:DV10 K10:DI10">
-    <cfRule type="expression" dxfId="49" priority="55">
+    <cfRule type="expression" dxfId="66" priority="75">
       <formula>AND(TODAY()&gt;=K$4,TODAY()&lt;L$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DJ10:DV10">
-    <cfRule type="expression" dxfId="48" priority="56" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="76" stopIfTrue="1">
       <formula>AND($C11="Low Risk",DJ$4&gt;=$H11,DJ$4&lt;=$H11+$I11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="77" stopIfTrue="1">
       <formula>AND($C11="High Risk",DJ$4&gt;=$H11,DJ$4&lt;=$H11+$I11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="58" stopIfTrue="1">
+    <cfRule type="expression" dxfId="63" priority="78" stopIfTrue="1">
       <formula>AND($C11="On Track",DJ$4&gt;=$H11,DJ$4&lt;=$H11+$I11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="62" priority="79" stopIfTrue="1">
       <formula>AND($C11="Med Risk",DJ$4&gt;=$H11,DJ$4&lt;=$H11+$I11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="60" stopIfTrue="1">
+    <cfRule type="expression" dxfId="61" priority="80" stopIfTrue="1">
       <formula>AND(LEN($C11)=0,DJ$4&gt;=$H11,DJ$4&lt;=$H11+$I11-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DN10:DQ10">
-    <cfRule type="expression" dxfId="43" priority="61">
+    <cfRule type="expression" dxfId="60" priority="81">
       <formula>AND(TODAY()&gt;=DN$4,TODAY()&lt;DS$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DJ10:DM10">
-    <cfRule type="expression" dxfId="42" priority="62">
+    <cfRule type="expression" dxfId="59" priority="82">
       <formula>AND(TODAY()&gt;=DJ$4,TODAY()&lt;DS$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10:DI10">
-    <cfRule type="expression" dxfId="41" priority="63" stopIfTrue="1">
+    <cfRule type="expression" dxfId="58" priority="83" stopIfTrue="1">
       <formula>AND($C11="Low Risk",K$4&gt;=$H10,K$4&lt;=$H10+$I11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="64" stopIfTrue="1">
+    <cfRule type="expression" dxfId="57" priority="84" stopIfTrue="1">
       <formula>AND($C11="High Risk",K$4&gt;=$H10,K$4&lt;=$H10+$I11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="65" stopIfTrue="1">
+    <cfRule type="expression" dxfId="56" priority="85" stopIfTrue="1">
       <formula>AND($C11="On Track",K$4&gt;=$H10,K$4&lt;=$H10+$I11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="66" stopIfTrue="1">
+    <cfRule type="expression" dxfId="55" priority="86" stopIfTrue="1">
       <formula>AND($C11="Med Risk",K$4&gt;=$H10,K$4&lt;=$H10+$I11-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="67" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="87" stopIfTrue="1">
       <formula>AND(LEN($C11)=0,K$4&gt;=$H10,K$4&lt;=$H10+$I11-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="dataBar" priority="39">
+    <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -30513,90 +30710,90 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DR12:DV12 K12:DI12">
-    <cfRule type="expression" dxfId="36" priority="40">
+    <cfRule type="expression" dxfId="53" priority="60">
       <formula>AND(TODAY()&gt;=K$4,TODAY()&lt;L$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DJ12:DV12">
-    <cfRule type="expression" dxfId="35" priority="41" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="61" stopIfTrue="1">
       <formula>AND($C13="Low Risk",DJ$4&gt;=$H13,DJ$4&lt;=$H13+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="42" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="62" stopIfTrue="1">
       <formula>AND($C13="High Risk",DJ$4&gt;=$H13,DJ$4&lt;=$H13+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="63" stopIfTrue="1">
       <formula>AND($C13="On Track",DJ$4&gt;=$H13,DJ$4&lt;=$H13+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="44" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="64" stopIfTrue="1">
       <formula>AND($C13="Med Risk",DJ$4&gt;=$H13,DJ$4&lt;=$H13+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="65" stopIfTrue="1">
       <formula>AND(LEN($C13)=0,DJ$4&gt;=$H13,DJ$4&lt;=$H13+$I13-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DN12:DQ12">
-    <cfRule type="expression" dxfId="30" priority="46">
+    <cfRule type="expression" dxfId="47" priority="66">
       <formula>AND(TODAY()&gt;=DN$4,TODAY()&lt;DS$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DJ12:DM12">
-    <cfRule type="expression" dxfId="29" priority="47">
+    <cfRule type="expression" dxfId="46" priority="67">
       <formula>AND(TODAY()&gt;=DJ$4,TODAY()&lt;DS$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:DI12">
-    <cfRule type="expression" dxfId="28" priority="48" stopIfTrue="1">
+    <cfRule type="expression" dxfId="45" priority="68" stopIfTrue="1">
       <formula>AND($C13="Low Risk",K$4&gt;=$H12,K$4&lt;=$H12+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="49" stopIfTrue="1">
+    <cfRule type="expression" dxfId="44" priority="69" stopIfTrue="1">
       <formula>AND($C13="High Risk",K$4&gt;=$H12,K$4&lt;=$H12+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="70" stopIfTrue="1">
       <formula>AND($C13="On Track",K$4&gt;=$H12,K$4&lt;=$H12+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="71" stopIfTrue="1">
       <formula>AND($C13="Med Risk",K$4&gt;=$H12,K$4&lt;=$H12+$I13-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="41" priority="72" stopIfTrue="1">
       <formula>AND(LEN($C13)=0,K$4&gt;=$H12,K$4&lt;=$H12+$I13-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CZ27:DV27">
-    <cfRule type="expression" dxfId="23" priority="2577" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="2597" stopIfTrue="1">
       <formula>AND($C30="Low Risk",CZ$4&gt;=$H30,CZ$4&lt;=$H30+$I30-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="2578" stopIfTrue="1">
+    <cfRule type="expression" dxfId="39" priority="2598" stopIfTrue="1">
       <formula>AND($C30="High Risk",CZ$4&gt;=$H30,CZ$4&lt;=$H30+$I30-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="2579" stopIfTrue="1">
+    <cfRule type="expression" dxfId="38" priority="2599" stopIfTrue="1">
       <formula>AND($C30="On Track",CZ$4&gt;=$H30,CZ$4&lt;=$H30+$I30-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="2580" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="2600" stopIfTrue="1">
       <formula>AND($C30="Med Risk",CZ$4&gt;=$H30,CZ$4&lt;=$H30+$I30-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="2581" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="2601" stopIfTrue="1">
       <formula>AND(LEN($C30)=0,CZ$4&gt;=$H30,CZ$4&lt;=$H30+$I30-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K27:DI27">
-    <cfRule type="expression" dxfId="18" priority="2587" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="2607" stopIfTrue="1">
       <formula>AND($C30="Low Risk",K$4&gt;=$H27,K$4&lt;=$H27+$I30-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="2588" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="2608" stopIfTrue="1">
       <formula>AND($C30="High Risk",K$4&gt;=$H27,K$4&lt;=$H27+$I30-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2589" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="2609" stopIfTrue="1">
       <formula>AND($C30="On Track",K$4&gt;=$H27,K$4&lt;=$H27+$I30-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="2590" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="2610" stopIfTrue="1">
       <formula>AND($C30="Med Risk",K$4&gt;=$H27,K$4&lt;=$H27+$I30-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="2591" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="2611" stopIfTrue="1">
       <formula>AND(LEN($C30)=0,K$4&gt;=$H27,K$4&lt;=$H27+$I30-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="dataBar" priority="31">
+    <cfRule type="dataBar" priority="51">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -30610,12 +30807,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K28:DV28">
-    <cfRule type="expression" dxfId="13" priority="32">
+    <cfRule type="expression" dxfId="30" priority="52">
       <formula>AND(TODAY()&gt;=K$4,TODAY()&lt;L$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -30629,52 +30826,102 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DR29:DV29 K29:DI29">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="29" priority="22">
       <formula>AND(TODAY()&gt;=K$4,TODAY()&lt;L$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DN29:DQ29">
-    <cfRule type="expression" dxfId="11" priority="8">
+    <cfRule type="expression" dxfId="28" priority="28">
       <formula>AND(TODAY()&gt;=DN$4,TODAY()&lt;DS$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DJ29:DM29">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="27" priority="29">
       <formula>AND(TODAY()&gt;=DJ$4,TODAY()&lt;DS$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13:DV13 K14:DI14">
-    <cfRule type="expression" dxfId="9" priority="2743" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="2763" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",K$4&gt;=$H13,K$4&lt;=$H13+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2744" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="2764" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",K$4&gt;=$H13,K$4&lt;=$H13+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="2745" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="2765" stopIfTrue="1">
       <formula>AND(#REF!="On Track",K$4&gt;=$H13,K$4&lt;=$H13+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2746" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="2766" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",K$4&gt;=$H13,K$4&lt;=$H13+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2747" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="2767" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,K$4&gt;=$H13,K$4&lt;=$H13+#REF!-1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DJ14:DV14">
-    <cfRule type="expression" dxfId="4" priority="2759" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="2779" stopIfTrue="1">
       <formula>AND(#REF!="Low Risk",DJ$4&gt;=#REF!,DJ$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2760" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="2780" stopIfTrue="1">
       <formula>AND(#REF!="High Risk",DJ$4&gt;=#REF!,DJ$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2761" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="2781" stopIfTrue="1">
       <formula>AND(#REF!="On Track",DJ$4&gt;=#REF!,DJ$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2762" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="2782" stopIfTrue="1">
       <formula>AND(#REF!="Med Risk",DJ$4&gt;=#REF!,DJ$4&lt;=#REF!+#REF!-1)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2763" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="2783" stopIfTrue="1">
       <formula>AND(LEN(#REF!)=0,DJ$4&gt;=#REF!,DJ$4&lt;=#REF!+#REF!-1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AZ28">
+    <cfRule type="expression" dxfId="9" priority="19">
+      <formula>AND(TODAY()&gt;=AZ$4,TODAY()&lt;BA$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AY28">
+    <cfRule type="expression" dxfId="8" priority="17">
+      <formula>AND(TODAY()&gt;=AY$4,TODAY()&lt;AZ$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BH28">
+    <cfRule type="expression" dxfId="7" priority="15">
+      <formula>AND(TODAY()&gt;=BH$4,TODAY()&lt;BI$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BI28">
+    <cfRule type="expression" dxfId="6" priority="13">
+      <formula>AND(TODAY()&gt;=BI$4,TODAY()&lt;BJ$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BJ28">
+    <cfRule type="expression" dxfId="5" priority="11">
+      <formula>AND(TODAY()&gt;=BJ$4,TODAY()&lt;BK$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BK28">
+    <cfRule type="expression" dxfId="4" priority="9">
+      <formula>AND(TODAY()&gt;=BK$4,TODAY()&lt;BL$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BL28">
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>AND(TODAY()&gt;=BL$4,TODAY()&lt;BM$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BM28">
+    <cfRule type="expression" dxfId="2" priority="5">
+      <formula>AND(TODAY()&gt;=BM$4,TODAY()&lt;BN$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BN28">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>AND(TODAY()&gt;=BN$4,TODAY()&lt;BO$4)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BN28">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(TODAY()&gt;=BN$4,TODAY()&lt;BO$4)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
@@ -30743,196 +30990,6 @@
           <xm:sqref>G145:G146</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="212" id="{81729095-AA92-410C-9893-CB15CD77272C}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>H171:I171 J93 DV95 DV92</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="207" id="{4F7B5DEF-CB34-455C-8948-2A733518504E}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>DJ53:DV53</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="205" id="{902E941D-F9A5-4BAB-AA67-6B688A391C39}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>DJ61:DV61</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="203" id="{23F9207C-1E0B-44DC-8C0C-355F9728E5F5}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>DJ66:DV66</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="201" id="{4698606C-6795-448C-BEB7-C6654E0124DE}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>DJ72:DV72</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="199" id="{8C2D9B03-CC2A-4604-BAD7-3B7BF754A66D}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>DV85</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="197" id="{6463E2B1-EE84-432B-81DB-88E99F01910E}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>DV90</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="196" id="{1C143CBB-5E04-4041-A85C-59F5878DEA46}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>DV99</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="129" id="{28B55561-C59B-49E6-A335-E7B3BDB8E358}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>CH8:DA8</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1985" id="{3AE3B37F-C23E-4137-BCF6-686F154BBBB1}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>DV121:DV123 DW7:EL7 DV125:DV127 DV129:DV131 DV133:DV135 DV137:DV139 DV141:DV143 DU145:DV147 DU149:DV150 DU144 DU148 DV100:DV119 DV91 DV86:DV89 DJ73:DV83 DJ67:DV71 DJ62:DV65 DJ54:DV60 DV96:DV98 DB8:FK8 DV93:DV94 K8:CG8 DJ32:DV52 K13:DV27 K144:DT150 DV84 DJ84:DU143 K32:DI66 CB67:DI67 K67:BZ67 BY68:DI68 K68:BW68 K69:DI143 K30:DV31</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6CF2FB1D-8D25-4911-8B09-C5F27E2E9E5E}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
@@ -30946,25 +31003,6 @@
             </x14:dataBar>
           </x14:cfRule>
           <xm:sqref>G11</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="113" id="{2E5FD8EF-9881-4175-B033-43E668064505}">
-            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>2</xm:f>
-              </x14:cfvo>
-              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
-              <x14:cfIcon iconSet="3Flags" iconId="1"/>
-              <x14:cfIcon iconSet="3Signs" iconId="0"/>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>K11:DV11</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A43E8637-D034-4238-9C99-E7FA7DA6F558}">
@@ -30997,7 +31035,261 @@
           <xm:sqref>G9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="76" id="{CF548F1B-0379-488E-B42D-9E8946AC789B}">
+          <x14:cfRule type="dataBar" id="{CCE2A728-F0B4-42A1-A3FE-B43A6BD8C8D4}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G12</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BCF4D11A-2CE7-4A95-B7EB-D3773D691236}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{1DD9ECA5-F474-4A43-9305-9D8710C0343D}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>G29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="232" id="{81729095-AA92-410C-9893-CB15CD77272C}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H171:I171 J93 DV95 DV92</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="227" id="{4F7B5DEF-CB34-455C-8948-2A733518504E}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>DJ53:DV53</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="225" id="{902E941D-F9A5-4BAB-AA67-6B688A391C39}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>DJ61:DV61</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="223" id="{23F9207C-1E0B-44DC-8C0C-355F9728E5F5}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>DJ66:DV66</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="221" id="{4698606C-6795-448C-BEB7-C6654E0124DE}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>DJ72:DV72</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="219" id="{8C2D9B03-CC2A-4604-BAD7-3B7BF754A66D}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>DV85</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="217" id="{6463E2B1-EE84-432B-81DB-88E99F01910E}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>DV90</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="216" id="{1C143CBB-5E04-4041-A85C-59F5878DEA46}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>DV99</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="149" id="{28B55561-C59B-49E6-A335-E7B3BDB8E358}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>CH8:DA8</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2005" id="{3AE3B37F-C23E-4137-BCF6-686F154BBBB1}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>DV121:DV123 DW7:EL7 DV125:DV127 DV129:DV131 DV133:DV135 DV137:DV139 DV141:DV143 DU145:DV147 DU149:DV150 DU144 DU148 DV100:DV119 DV91 DV86:DV89 DJ73:DV83 DJ67:DV71 DJ62:DV65 DJ54:DV60 DV96:DV98 DB8:FK8 DV93:DV94 K8:CG8 DJ32:DV52 K13:DV27 K144:DT150 DV84 DJ84:DU143 K32:DI66 CB67:DI67 K67:BZ67 BY68:DI68 K68:BW68 K69:DI143 K30:DV31</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="133" id="{2E5FD8EF-9881-4175-B033-43E668064505}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K11:DV11</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="96" id="{CF548F1B-0379-488E-B42D-9E8946AC789B}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -31016,7 +31308,7 @@
           <xm:sqref>K9:DV9</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="68" id="{6219A49B-4DE0-45B5-901D-DC5D2E193BE4}">
+          <x14:cfRule type="iconSet" priority="88" id="{6219A49B-4DE0-45B5-901D-DC5D2E193BE4}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -31035,22 +31327,7 @@
           <xm:sqref>K10:DV10</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{CCE2A728-F0B4-42A1-A3FE-B43A6BD8C8D4}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>G12</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="53" id="{EEC7D114-B759-44EF-BF74-AE6E2A439ED2}">
+          <x14:cfRule type="iconSet" priority="73" id="{EEC7D114-B759-44EF-BF74-AE6E2A439ED2}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -31069,22 +31346,7 @@
           <xm:sqref>K12:DV12</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{BCF4D11A-2CE7-4A95-B7EB-D3773D691236}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>G28</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="38" id="{15B1211D-254B-4753-BBF6-A6A051D9A2E2}">
+          <x14:cfRule type="iconSet" priority="58" id="{15B1211D-254B-4753-BBF6-A6A051D9A2E2}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -31103,22 +31365,7 @@
           <xm:sqref>K28:DV28</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{1DD9ECA5-F474-4A43-9305-9D8710C0343D}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>G29</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="15" id="{064BC8E8-D86D-4A86-A7D4-7A5F8A158C60}">
+          <x14:cfRule type="iconSet" priority="35" id="{064BC8E8-D86D-4A86-A7D4-7A5F8A158C60}">
             <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -31136,6 +31383,196 @@
           </x14:cfRule>
           <xm:sqref>K29:DV29</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="20" id="{FA5209F2-FFB3-48A2-9A75-C5F48444F6B3}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>AZ28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="18" id="{9569EA1E-45EA-41F6-8DCD-BBB378E7F0DB}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>AY28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="16" id="{C1CDF43F-5FB1-436E-B1A0-C837108881E7}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>BH28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="14" id="{2C20F5C0-A864-455C-BF7A-1F3B0E897481}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>BI28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="12" id="{9A124741-B619-456B-9432-4C249064419D}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>BJ28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="10" id="{9E4406B4-555B-46BB-91BA-8F41101EBF4A}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>BK28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="8" id="{0A19B949-DB06-4FD9-A879-F135021CE80D}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>BL28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="6" id="{50F1ABC3-7A50-4B59-8E9D-37C10E1D63AF}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>BM28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{4665DCC6-FFD2-4A86-A5C0-13C97BC83B23}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>BN28</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{4B89AB24-9913-4F1E-83C7-3D670527242A}">
+            <x14:iconSet iconSet="3Stars" showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>BN28</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>